<commit_message>
update report and db
</commit_message>
<xml_diff>
--- a/apps/report_zap/zap_report.xlsx
+++ b/apps/report_zap/zap_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProject\tool\python_tool\apps\report_zap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick Wu\PycharmProjects\github\python_tool\apps\report_zap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F545AAE-FBF8-402A-A5D7-19C347DE0A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD04B675-53F7-466F-8EC5-0D0F10CA4918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zap_report" sheetId="1" r:id="rId1"/>
@@ -407,11 +407,6 @@
   </si>
   <si>
     <t>路徑遍尋</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>We detected that your website is vulnerable to dirctory traversal.
- A directory traversal attack allows an attacker access to arbritrary restricted files directories and sensitive commands by manipulating a url. Any device that exposes an http-based interface is potentially vulnerable to path traversal. This vulnerability allows attackers to read sensitive information within the websites restricted files, and may lead to data exposure, credential leakage, and accont compromise. Attackers may utilize special-characters sequences, for example the ../ special-character sequence, to alter the resource location requested in the url. Advanced information： Although most popular web servers will prevent this technique with security filters, attackers may bypass them using alternate encodings, including unicode-encoded slash characters, url encoded characters, and double url encodings. Even if the web server properly restricts path traversal attempts in the url path, a web application may still be vulnerable due to improper handling of user-supplied input, such as substituting the original url parameter value with the file name of one of the web application's dynamic scripts. Consequently the results can reveal source code because the file is interpreted as text instead of an executable script. These techniques often employ additional special characters such as the dot (.) to reveal the listing of the current working directory or %00 null characters in order to bypass rudimentary file extension checks.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -556,10 +551,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Open redirects are one of the OWASP 2010 Top Ten vulnerabilities. This check looks at user-supplied input in query string parameters and POST data to identify where open redirects might be possible. Open redirects occur when an application allows user-supplied input (e.g. http：//nottrusted.com) to control an offsite redirect. This is generally a pretty accurate way to find where 301 or 302 redirects could be exploited by spammers or phishing attacks. For example an attacker could supply a user with the following link： http：//example.com/example.php?url=http：//malicious.example.com.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>To avoid the open redirect vulnerability, parameters of the application  script/program must be validated before sending 302 HTTP code (redirect) to the client browser. Implement safe redirect functionality that only redirects to relative URI's, or a list of trusted domains</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -569,11 +560,6 @@
   </si>
   <si>
     <t>文件引用（遠端文件）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remote File Include (RFI) is an attack technique used to exploit “dynamic file include” mechanisms in web applications. When web applications take user input (URL, parameter value, etc.) and pass them into file include
- commands, the web application might be tricked into including remote files with malicious code. Almost all web application frameworks support file inclusion. File inclusion is mainly used for packaging common code into separate files that are later referenced by main application modules. When a web application references an include file, the code in this file may be executed implicitly or explicitly by calling specific procedures. If the choice of module to load is based on elements from the HTTP request, the web application might be vulnerable to RFI. An attacker can use RFI for： * Running malicious code on the server： any code in the included malicious files will be run by the server. If the file include is not executed using some wrapper, code in include files is executed in the context of the server user. This could lead to a complete system compromise. * Running malicious code on clients： the attacker's malicious code can manipulate the content of the response sent to the client. The attacker can embed malicious code in the response that will be run by the client (for example, JavaScript to steal the client session cookies). PHP is particularly vulnerable to RFI attacks due to the extensive use of “file includes” in PHP programming and due to default server configurations that increase susceptibility to an RFI attack.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -729,23 +715,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Misconfigured Headers： CORS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>標頭配置錯誤（CORS）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>We detected that your website has misconfigured CORS headers.
- Due to a misconfigured 'Access-Control-Allow-Origin： *' header on the web server and third party resource loading in the webpage, the victim's browser may load malicious resources and execute harmful scripts. Impact includes credential theft, data leakage, and phishing attempts. Cross-Origin Resource Sharing (CORS) is an HTTP-header based mechanism that allows a server to indicate any other origins (domain, protocol, or port) than its own from which a browser should permit loading of resources. This helps restrict the loaded data to trusted sources and prevent the browser from loading malicious external content. Thus, setting a wildcard directive ('*') nulls the protection from CORS settings.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>檢測到您的網站可能有會產生安全疑慮的CORS配置錯誤。常見於設置了「 Access-Control-Allow-Origin: *」，同時網頁引用的第三方網頁中包含XSS或CSRF程式碼，則會導致自身的網頁受到第三方網頁中的惡意程式攻擊。 跨域資源共享（CORS）是一種基於HTTP標頭的機制，它允許伺服器指示瀏覽器應允許加載的資源外的其他任何來源（域，協議或端口），若Web服務器上的“ Access-Control-Allow-Origin”標頭配置錯誤，可能會加載異常或惡意的Web瀏覽器數據。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Cross-Domain Misconfiguration</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -755,10 +728,6 @@
   </si>
   <si>
     <t>標頭配置錯誤（CSP）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misconfigured Headers： CSP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -772,10 +741,6 @@
   </si>
   <si>
     <t>Proxy Disclosure</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Insecure HTTP Method： TRACE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -924,10 +889,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Misconfigured Headers： Missing CSP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Content Security Policy (CSP) is an added layer of security that helps to detect and mitigate certain types of attacks, including Cross Site Scripting (XSS) and data injection attacks. These attacks are used for everything from data theft to site defacement or distribution of malware. CSP provides a set of standard HTTP headers that allow website owners to declare approved sources of content that browsers should be allowed to load on that page — covered types are JavaScript, CSS, HTML frames, fonts, images and embeddable objects such as Java applets, ActiveX, audio and video files.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -941,10 +902,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Misconfigured Cookie： Missing SameSite Attribute</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>A cookie has been set without the SameSite attribute, which means  that the cookie can be sent as a result of a ‘cross-site’ request. The SameSite attribute is an effective counter measure to cross-site request forgery, cross-site script inclusion, and timing attacks.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -954,10 +911,6 @@
   </si>
   <si>
     <t>X-Content-Type-Options Header Missing</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misconfigured Headers： Missing X-Content-Type-Options</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -974,10 +927,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Cross-Domain File Inclusion： Javascript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>跨域引用檔案（Javascript）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1007,10 +956,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Header Leakage： X-Powered-By</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>標頭資訊洩露（X-Powered-By）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1027,10 +972,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Header Leakage： X-AspNet-Version</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>標頭資訊洩露（X-AspNet-Version）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1040,11 +981,6 @@
   </si>
   <si>
     <t>檢測到您的網站在標頭中洩漏X-AspNet-Version信息，該信息可能會洩露後端伺服器資訊以及ASP.NET版本，造成安全風險。攻擊者可比照各種軟韌體版本資訊找出過期或未修補的系統，進而滲透利用。即使當前版本安全，未來若此版本有新漏洞釋出，您的網站可能因洩漏此資訊而在短時間內遭到攻擊。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remove the X-AspNet-Version HTTP header. To configure this 
-on Apache： Add this line in httpd.conf： Header unset X-AspNet-Version To configure this on nginx： Add this line in the location section in nginx.conf： proxy_hide_header X-AspNet-Version; To configure this on IIS： In the Application_PreSendRequestHeaders() function in Global.asax, add the folowing： response.Headers.remove(""X-AspNet-Version"") To configure this in HAProxy： Add the following line to HAProxy's config： http-response del-header X-AspNet-Version</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1152,10 +1088,6 @@
   </si>
   <si>
     <t>檢測到您的網站在不安全的連接上使用HTTP基本身份驗證，這可能會產生安全風險。 使攻擊者可以輕易的攔截登錄憑證，並將其憑證在其他主機重放，誘騙用戶將憑據提供給錯誤的位置。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Buffer Overflow： Integer Overflow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1286,10 +1218,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Misconfigured Headers： Missing Strict-Transport-Security</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>HTTP Strict Transport Security (HSTS) is a web security policy
  mechanism whereby a web server declares that complying user agents (such as a web browser) are to interact with it using only secure HTTPS connections (i.e. HTTP layered over TLS/SSL). HSTS is an IETF standards track protocol and is specified in RFC 6797.</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1299,13 +1227,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Misconfigured Cookie： Missing HttpOnly Attribute</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misconfigured Cookie： Missing Secure Attribute</t>
-  </si>
-  <si>
     <t>標頭配置錯誤（缺少 HttpOnly 屬性）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1326,10 +1247,6 @@
   </si>
   <si>
     <t>標頭配置錯誤（缺少 Cache-control and Pragma）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misconfigured Headers： Missing Cache-control and Pragma</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1392,10 +1309,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Misconfigured Headers： X-Backend-Server</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>標頭配置錯誤（X-Backend-Server）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1437,10 +1350,6 @@
   </si>
   <si>
     <t>未被採用的 cookie</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Repeated GET requests： drop a different cookie each time, followed by normal request with all cookies to stabilize session, compare responses against original baseline GET. This can reveal areas where cookie based authentication/attributes are not actually enforced.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1560,16 +1469,6 @@
     <t>• 確保只從受信任的來源及域載入JavaScript文件 將所有應用程序文件託管在伺服器或直得信任的第三方服務（例如CDN）。</t>
   </si>
   <si>
-    <t xml:space="preserve">• 'X-Frame-Options： DENY' completely denies to be loaded in frame/iframe. In /etc/apache2/conf-enabled/security.conf (debian) or /etc/httpd/conf/httpd.conf (redhat), add the entry： Header set X-Frame-Options： DENY 
-• 'X-Frame-Options： SAMEORIGIN' allows only if the site which wants to load has a same origin. In /etc/apache2/conf-enabled/security.conf (debian) or /etc/httpd/conf/httpd.conf (redhat), add the entry： Header set X-Frame-Options： SAMEORIGIN 
-</t>
-  </si>
-  <si>
-    <t>• 如果您的網站不須使用X-Frame，請將X-Frame-Options設定為DENY，以預防攻擊者利用X-Frame攻擊。
-以常見的網站伺服器Apache為例，請在security.conf中新增一行設定「Header set X-Frame-Options: "DENY"」，其他網站伺服器請參考相關安全性設定。
-• 如果您的網站會用到來自內部的X-Frame，請將X-Frame-Options設定為SAMEORIGIN，以防止從外部嵌入的X-Frame。以常見的網站伺服器Apache為例，請在security.conf中新增一行設定「Header set X-Frame-Options: "SAMEORIGIN"」，其他網站伺服器請參考相關安全性設定。</t>
-  </si>
-  <si>
     <t>• 在您的WebServer設定一個帶有'nosniff'值的'X-Content-Type-Options'標頭。</t>
   </si>
   <si>
@@ -1596,15 +1495,6 @@
 • 移除或隱藏所有網頁上檢測到的非公開的電子郵件。
 • 請驗證所檢測的IP位置是否為機密信息。 
 • 移除或隱藏所有網頁上檢測到的非公開的IP位置。</t>
-  </si>
-  <si>
-    <t>• Find the location of Apache's main configuration file 'apache2.conf', usually under '/etc/apache2/apache2.conf'. 
-• Edit this file with root access to your server, and modify this line by adding a preceding '-' sign to the word 'Indexes'： 'Options Indexes FollowSymLinks' change to 'Options -Indexes FollowSymLinks' • Save the file and restart Apache Alternatively, edit the '.htaccess' and modify the Options line as 'Options -Indexes</t>
-  </si>
-  <si>
-    <t>• 查找Apache主要配置文件" apache2.conf”的位置，通常在“ /etc/apache2/apache2.conf”下。 
-• 使用對服務器的root訪問權限來編輯此文件，並通過在單詞“索引”中添加前面的“-”符號來修改此行： '選項索引FollowSymLinks'更改為'選項-索引FollowSymLinks' 。
-• 保存文件並重新啟動Apache 或者，編輯“ .htaccess”並將“選項”行修改為“選項-索引””</t>
   </si>
   <si>
     <t>• If possible, update to OpenSSL 1.0.1g or later. 
@@ -1629,25 +1519,8 @@
 etc. is configured to enforce Strict-Transport-Security.</t>
   </si>
   <si>
-    <t>• 在您的WebServer設定一個Strict-Transport-Security： max-age=31536000; includeSubDomains的標頭 ＊此設定會導致只能通過HTTP進行服務的頁面的訪問失敗。</t>
-  </si>
-  <si>
-    <t>•Remove the X-Powered-By HTTP header. To configure this on Apache： Add these lines in httpd.conf： &lt;IfModule mod_headers.c&gt; Header unset X-Powered-By &lt;/IfModule&gt; To configure this on nginx： Add this line in nginx.conf： proxy_hide_header X-Powered-By; Additionally, you must also modify the configuration for used languages(ex： PHP) and framework(ex： Tomcat) to remove the X-Powered-By header. To configure this on IIS： Change the system.webSerer section in Web.config as below： &lt;system.webServer&gt;</t>
-  </si>
-  <si>
     <t>• 在IIS伺服器中的Web.config修改system.webServer區段：
 &lt;httpProtocol&gt;&lt;customHeaders&gt;&lt;remove name="X-Powered-By" /&gt;&lt;/customHeaders&gt;&lt;/httpProtocol&gt;&lt;/system.webServer&gt;</t>
-  </si>
-  <si>
-    <t>•Ensure that your web server, application server, load balancer, etc. is configured to set the Content-Security-Policy header, to achieve optimal browser support： 'Content-Security-Policy' for Chrome 25+, Firefox 23+ and Safari 7+, 'X-Content-Security-Policy' for Firefox 4.0+ and Internet Explorer 10+, and 'X-WebKit-CSP' for Chrome 14+ and Safari 6+</t>
-  </si>
-  <si>
-    <t>• 限制外部連入的檔案和禁用inline語法，這是預設全部阻擋的寫法，也是最嚴格最安全的方案，設定範例如下
-content-security-policy: default-src 'none';
-• 增加外部連入的白名單，限制外部連入的來源，請避免在來源url中使用「*」，設定範例如下
-content-security-policy: default-src 'none'; 
-script-src 'self' https://www.google.com;
-• 避免在CSP設定中使用「unsafe-inline」</t>
   </si>
   <si>
     <t>• The best strategy to avoid mixed content blocking is to serve all the content as HTTPS instead of HTTP. A page that is available over SSL/TLS must be comprised completely of content which is transmitted over SSL/TLS. 
@@ -1693,17 +1566,6 @@
     <t>• SameSite有三個數值 — Strict、Lax和None建議依據網站需求參考Strict＆Lax進行設定Strict Strict的要求最為嚴格，完全禁止第三方Cookies，只有當前網頁的 URL與請求目標一致，才會送出Cookie。 這個規則非常嚴格，適合用於銀行需要交易的網站中，保障客戶資料的安全。Lax Lax的要求則較為寬鬆，大多數情況也是不發送Cookie到第三方 ，但是Get請求除外。 這是一個平衡網路安全和使用者體驗的做法。由於Cookies可以跨網站發送，而風險較高的要求，例如POST，在Lax的設定下將會被禁止，阻止cross-site request forgery attacks 進行。</t>
   </si>
   <si>
-    <t>• To prevent the use of 'unsafe-inline' but still use inline scripts and styles on a page, consider converting them to safe sources via nonces or hashes. 
-• For example, using the nonce-source you may specify inline style blocks with： ""Content-Security-Policy： style-src 'nonce-2726c7f26c'"" and set the same nonce on the style element： '&lt;style nonce=""2726c7f26c""&gt; #inline-style { background： red; } &lt;/style&gt;' • Hash-source inline styles can be achieved similarly.</t>
-  </si>
-  <si>
-    <t>• 移除X-AspNet-Version標頭。 
-• 設定Apache 在 httpd.conf中加入一行：Header unset X-AspNet-Version
-• 設定nginx在 nginx.conf的location區段中加入一行：proxy_hide_header X-AspNet-Version;
-• 設定 IIS在Global.asax的 Application_PreSendRequestHeaders()裡加入一行：response.Headers.remove("X-AspNet-Version") 
-• 設定HAProxy在HAProxy前端組態設定中加入一行： http-response del-header X-AspNet-Version。</t>
-  </si>
-  <si>
     <t xml:space="preserve">• If the application does not require cross-origin requests, check that no policy is set. 
 • The 'Access-Control-Allow-Origin' header should never be set to '*' or 'null', unless the whole content of the application is made to be public. Always ensure that it allows the most specific and restrictive set of domains. </t>
   </si>
@@ -1726,10 +1588,6 @@
 • 默認情況下不允許跨域身份驗證請求，如果父站點需要跨域身份驗證，則應通過CSP或類似的站點策略定義允許進行身份驗證的域白名單。 
 • 將所有內網內容列入白名單或代理，以阻止惡意身份驗證請求。 
 • 確保身份驗證token的安全並設置較短的到期時間。</t>
-  </si>
-  <si>
-    <t>• Add 'rel=""noopener noreferrer""' to every 'a'-element that has 'target=""_blank""'. 'noopener' ensures that the linked page does not have access to 'window.opener' from the linking page. 'noreferrer' makes sure that the request referrer header is not being sent. This is supported by most recent versions of modern browsers, with Internet Explorer being an exception. • If you are using JavaScript, the following achieves the same： 'var myNewWindow = window.open(url, name, ""noopener,noreferrer"") myNewWindow.opener = null' 
-• If you show user-generated content on your page you must sanitize the input and apply ""noopener noreferrer"" to every link.</t>
   </si>
   <si>
     <t>• 將html中所有用到開新視窗的跳轉連結加上noopener與noreferrer設定，以跳轉至google為例
@@ -1833,16 +1691,6 @@
 •限制用戶對資料庫的存取權限，僅給予最低能滿足需求的權限，進而減少此攻擊對資料庫的危害。</t>
   </si>
   <si>
-    <t>• Hide or remove Trace.axd in production stages. 
-• Disable the Trace Viewer unless it is actually required in development. Ensure access to it requires authentication and authorization. 
-• To disable ASP.NET tracing, apply the following changes to your web.config file： &lt;System.Web&gt; &lt;trace enabled=""false"" /&gt; &lt;/System.Web&gt;</t>
-  </si>
-  <si>
-    <t>• 應將此文件隱藏或從生產階段中刪除，因為它可能洩漏大量信息。 
-• 請考慮研發過程中是否實際需要Trace Viewer，如果不需要，則將其禁用。 
-• 若不禁用，請確保任何人進行存取時需要身份驗證和授權。 要禁用ASP.NET跟踪，請將以下更改應用於web.config文件： &lt;System.Web&gt; &lt;trace enabled=""false"" /&gt; &lt;/System.Web&gt;。</t>
-  </si>
-  <si>
     <t>• 確認網站上.htaccess 檔案的存取權限，確保使用者無法下載.htaccess 。
 • 設定完成後以報告中路徑測試，再次確認使用者無法存取檔案</t>
   </si>
@@ -1876,13 +1724,144 @@
   <si>
     <t>• 將流量代理到已知上游Server，通過IP地址或DNS名稱來標識Server進行過濾。 
 • 在NGINX配置中或使用Web應用程序防火牆（WAF），將所有帶有異常標頭值的請求丟棄。</t>
+  </si>
+  <si>
+    <t>We detected that your website is vulnerable to dirctory traversal.
+ A directory traversal attack allows an attacker access to arbritrary restricted files directories and sensitive commands by manipulating a url. Any device that exposes an http-based interface is potentially vulnerable to path traversal. This vulnerability allows attackers to read sensitive information within the websites restricted files, and may lead to data exposure, credential leakage, and accont compromise. Attackers may utilize special-characters sequences, for example the ../ special-character sequence, to alter the resource location requested in the url. Advanced information：Although most popular web servers will prevent this technique with security filters, attackers may bypass them using alternate encodings, including unicode-encoded slash characters, url encoded characters, and double url encodings. Even if the web server properly restricts path traversal attempts in the url path, a web application may still be vulnerable due to improper handling of user-supplied input, such as substituting the original url parameter value with the file name of one of the web application's dynamic scripts. Consequently the results can reveal source code because the file is interpreted as text instead of an executable script. These techniques often employ additional special characters such as the dot (.) to reveal the listing of the current working directory or %00 null characters in order to bypass rudimentary file extension checks.</t>
+  </si>
+  <si>
+    <t>Remote File Include (RFI) is an attack technique used to exploit “dynamic file include” mechanisms in web applications. When web applications take user input (URL, parameter value, etc.) and pass them into file include
+ commands, the web application might be tricked into including remote files with malicious code. Almost all web application frameworks support file inclusion. File inclusion is mainly used for packaging common code into separate files that are later referenced by main application modules. When a web application references an include file, the code in this file may be executed implicitly or explicitly by calling specific procedures. If the choice of module to load is based on elements from the HTTP request, the web application might be vulnerable to RFI. An attacker can use RFI for：* Running malicious code on the server：any code in the included malicious files will be run by the server. If the file include is not executed using some wrapper, code in include files is executed in the context of the server user. This could lead to a complete system compromise. * Running malicious code on clients：the attacker's malicious code can manipulate the content of the response sent to the client. The attacker can embed malicious code in the response that will be run by the client (for example, JavaScript to steal the client session cookies). PHP is particularly vulnerable to RFI attacks due to the extensive use of “file includes” in PHP programming and due to default server configurations that increase susceptibility to an RFI attack.</t>
+  </si>
+  <si>
+    <t>Misconfigured Cookie：Missing HttpOnly Attribute</t>
+  </si>
+  <si>
+    <t>Misconfigured Cookie：Missing Secure Attribute</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：Missing Cache-control and Pragma</t>
+  </si>
+  <si>
+    <t>Cross-Domain File Inclusion：Javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• 'X-Frame-Options：DENY' completely denies to be loaded in frame/iframe. In /etc/apache2/conf-enabled/security.conf (debian) or /etc/httpd/conf/httpd.conf (redhat), add the entry：Header set X-Frame-Options：DENY 
+• 'X-Frame-Options：SAMEORIGIN' allows only if the site which wants to load has a same origin. In /etc/apache2/conf-enabled/security.conf (debian) or /etc/httpd/conf/httpd.conf (redhat), add the entry：Header set X-Frame-Options：SAMEORIGIN 
+</t>
+  </si>
+  <si>
+    <t>• 如果您的網站不須使用X-Frame，請將X-Frame-Options設定為DENY，以預防攻擊者利用X-Frame攻擊。
+以常見的網站伺服器Apache為例，請在security.conf中新增一行設定「Header set X-Frame-Options："DENY"」，其他網站伺服器請參考相關安全性設定。
+• 如果您的網站會用到來自內部的X-Frame，請將X-Frame-Options設定為SAMEORIGIN，以防止從外部嵌入的X-Frame。以常見的網站伺服器Apache為例，請在security.conf中新增一行設定「Header set X-Frame-Options："SAMEORIGIN"」，其他網站伺服器請參考相關安全性設定。</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：Missing X-Content-Type-Options</t>
+  </si>
+  <si>
+    <t>Open redirects are one of the OWASP 2010 Top Ten vulnerabilities. This check looks at user-supplied input in query string parameters and POST data to identify where open redirects might be possible. Open redirects occur when an application allows user-supplied input (e.g. http：//nottrusted.com) to control an offsite redirect. This is generally a pretty accurate way to find where 301 or 302 redirects could be exploited by spammers or phishing attacks. For example an attacker could supply a user with the following link：http：//example.com/example.php?url=http：//malicious.example.com.</t>
+  </si>
+  <si>
+    <t>• Find the location of Apache's main configuration file 'apache2.conf', usually under '/etc/apache2/apache2.conf'. 
+• Edit this file with root access to your server, and modify this line by adding a preceding '-' sign to the word 'Indexes'：'Options Indexes FollowSymLinks' change to 'Options -Indexes FollowSymLinks' • Save the file and restart Apache Alternatively, edit the '.htaccess' and modify the Options line as 'Options -Indexes</t>
+  </si>
+  <si>
+    <t>• 查找Apache主要配置文件" apache2.conf”的位置，通常在“ /etc/apache2/apache2.conf”下。 
+• 使用對服務器的root訪問權限來編輯此文件，並通過在單詞“索引”中添加前面的“-”符號來修改此行：'選項索引FollowSymLinks'更改為'選項-索引FollowSymLinks' 。
+• 保存文件並重新啟動Apache 或者，編輯“ .htaccess”並將“選項”行修改為“選項-索引””</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：Missing Strict-Transport-Security</t>
+  </si>
+  <si>
+    <t>• 在您的WebServer設定一個Strict-Transport-Security：max-age=31536000; includeSubDomains的標頭 ＊此設定會導致只能通過HTTP進行服務的頁面的訪問失敗。</t>
+  </si>
+  <si>
+    <t>Header Leakage：X-Powered-By</t>
+  </si>
+  <si>
+    <t>•Remove the X-Powered-By HTTP header. To configure this on Apache：Add these lines in httpd.conf：&lt;IfModule mod_headers.c&gt; Header unset X-Powered-By &lt;/IfModule&gt; To configure this on nginx：Add this line in nginx.conf：proxy_hide_header X-Powered-By; Additionally, you must also modify the configuration for used languages(ex：PHP) and framework(ex：Tomcat) to remove the X-Powered-By header. To configure this on IIS：Change the system.webSerer section in Web.config as below：&lt;system.webServer&gt;</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：Missing CSP</t>
+  </si>
+  <si>
+    <t>•Ensure that your web server, application server, load balancer, etc. is configured to set the Content-Security-Policy header, to achieve optimal browser support：'Content-Security-Policy' for Chrome 25+, Firefox 23+ and Safari 7+, 'X-Content-Security-Policy' for Firefox 4.0+ and Internet Explorer 10+, and 'X-WebKit-CSP' for Chrome 14+ and Safari 6+</t>
+  </si>
+  <si>
+    <t>• 限制外部連入的檔案和禁用inline語法，這是預設全部阻擋的寫法，也是最嚴格最安全的方案，設定範例如下
+content-security-policy：default-src 'none';
+• 增加外部連入的白名單，限制外部連入的來源，請避免在來源url中使用「*」，設定範例如下
+content-security-policy：default-src 'none'; 
+script-src 'self' https://www.google.com;
+• 避免在CSP設定中使用「unsafe-inline」</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：X-Backend-Server</t>
+  </si>
+  <si>
+    <t>Misconfigured Cookie：Missing SameSite Attribute</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：CSP</t>
+  </si>
+  <si>
+    <t>• To prevent the use of 'unsafe-inline' but still use inline scripts and styles on a page, consider converting them to safe sources via nonces or hashes. 
+• For example, using the nonce-source you may specify inline style blocks with：""Content-Security-Policy：style-src 'nonce-2726c7f26c'"" and set the same nonce on the style element：'&lt;style nonce=""2726c7f26c""&gt; #inline-style { background：red; } &lt;/style&gt;' • Hash-source inline styles can be achieved similarly.</t>
+  </si>
+  <si>
+    <t>Header Leakage：X-AspNet-Version</t>
+  </si>
+  <si>
+    <t>Remove the X-AspNet-Version HTTP header. To configure this 
+on Apache：Add this line in httpd.conf：Header unset X-AspNet-Version To configure this on nginx：Add this line in the location section in nginx.conf：proxy_hide_header X-AspNet-Version; To configure this on IIS：In the Application_PreSendRequestHeaders() function in Global.asax, add the folowing：response.Headers.remove(""X-AspNet-Version"") To configure this in HAProxy：Add the following line to HAProxy's config：http-response del-header X-AspNet-Version</t>
+  </si>
+  <si>
+    <t>• 移除X-AspNet-Version標頭。 
+• 設定Apache 在 httpd.conf中加入一行：Header unset X-AspNet-Version
+• 設定nginx在 nginx.conf的location區段中加入一行：proxy_hide_header X-AspNet-Version;
+• 設定 IIS在Global.asax的 Application_PreSendRequestHeaders()裡加入一行：response.Headers.remove("X-AspNet-Version") 
+• 設定HAProxy在HAProxy前端組態設定中加入一行：http-response del-header X-AspNet-Version。</t>
+  </si>
+  <si>
+    <t>Misconfigured Headers：CORS</t>
+  </si>
+  <si>
+    <t>We detected that your website has misconfigured CORS headers.
+ Due to a misconfigured 'Access-Control-Allow-Origin：*' header on the web server and third party resource loading in the webpage, the victim's browser may load malicious resources and execute harmful scripts. Impact includes credential theft, data leakage, and phishing attempts. Cross-Origin Resource Sharing (CORS) is an HTTP-header based mechanism that allows a server to indicate any other origins (domain, protocol, or port) than its own from which a browser should permit loading of resources. This helps restrict the loaded data to trusted sources and prevent the browser from loading malicious external content. Thus, setting a wildcard directive ('*') nulls the protection from CORS settings.</t>
+  </si>
+  <si>
+    <t>檢測到您的網站可能有會產生安全疑慮的CORS配置錯誤。常見於設置了「 Access-Control-Allow-Origin：*」，同時網頁引用的第三方網頁中包含XSS或CSRF程式碼，則會導致自身的網頁受到第三方網頁中的惡意程式攻擊。 跨域資源共享（CORS）是一種基於HTTP標頭的機制，它允許伺服器指示瀏覽器應允許加載的資源外的其他任何來源（域，協議或端口），若Web服務器上的“ Access-Control-Allow-Origin”標頭配置錯誤，可能會加載異常或惡意的Web瀏覽器數據。</t>
+  </si>
+  <si>
+    <t>• Add 'rel=""noopener noreferrer""' to every 'a'-element that has 'target=""_blank""'. 'noopener' ensures that the linked page does not have access to 'window.opener' from the linking page. 'noreferrer' makes sure that the request referrer header is not being sent. This is supported by most recent versions of modern browsers, with Internet Explorer being an exception. • If you are using JavaScript, the following achieves the same：'var myNewWindow = window.open(url, name, ""noopener,noreferrer"") myNewWindow.opener = null' 
+• If you show user-generated content on your page you must sanitize the input and apply ""noopener noreferrer"" to every link.</t>
+  </si>
+  <si>
+    <t>Buffer Overflow：Integer Overflow</t>
+  </si>
+  <si>
+    <t>Insecure HTTP Method：TRACE</t>
+  </si>
+  <si>
+    <t>• Hide or remove Trace.axd in production stages. 
+• Disable the Trace Viewer unless it is actually required in development. Ensure access to it requires authentication and authorization. 
+• To disable ASP.NET tracing, apply the following changes to your web.config file：&lt;System.Web&gt; &lt;trace enabled=""false"" /&gt; &lt;/System.Web&gt;</t>
+  </si>
+  <si>
+    <t>• 應將此文件隱藏或從生產階段中刪除，因為它可能洩漏大量信息。 
+• 請考慮研發過程中是否實際需要Trace Viewer，如果不需要，則將其禁用。 
+• 若不禁用，請確保任何人進行存取時需要身份驗證和授權。 要禁用ASP.NET跟踪，請將以下更改應用於web.config文件：&lt;System.Web&gt; &lt;trace enabled=""false"" /&gt; &lt;/System.Web&gt;。</t>
+  </si>
+  <si>
+    <t>Repeated GET requests：drop a different cookie each time, followed by normal request with all cookies to stabilize session, compare responses against original baseline GET. This can reveal areas where cookie based authentication/attributes are not actually enforced.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2840,7 +2819,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2850,25 +2829,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="16.149999999999999"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="55.625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="10.625" style="1" customWidth="1"/>
-    <col min="7" max="12" width="55.625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.75" style="1"/>
+    <col min="1" max="2" width="8.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55.59765625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="12" width="55.59765625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2877,10 +2856,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -2901,12 +2880,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2915,12 +2894,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -2929,12 +2908,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -2943,12 +2922,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="363" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="370.9">
       <c r="A5" s="1">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -2957,10 +2936,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>120</v>
@@ -2969,24 +2948,24 @@
         <v>121</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>122</v>
+        <v>378</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="396" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="403.15">
       <c r="A6" s="1">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2995,33 +2974,33 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="K6" s="2" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -3030,12 +3009,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="80.650000000000006">
       <c r="A8" s="1">
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -3044,36 +3023,36 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="177.4">
       <c r="A9" s="1">
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -3082,68 +3061,68 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="49.5" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="64.5">
       <c r="A10" s="1">
         <v>10003</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="99" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="96.75">
       <c r="A11" s="1">
         <v>10010</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -3152,36 +3131,36 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>294</v>
+        <v>380</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="66" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="80.650000000000006">
       <c r="A12" s="1">
         <v>10011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -3190,36 +3169,36 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>295</v>
+        <v>381</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="99" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="96.75">
       <c r="A13" s="1">
         <v>10015</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>19</v>
@@ -3228,36 +3207,36 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>302</v>
+        <v>382</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="99" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="96.75">
       <c r="A14" s="1">
         <v>10017</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -3266,36 +3245,36 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>223</v>
+        <v>383</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>10019</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -3304,12 +3283,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="264" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="258">
       <c r="A16" s="1">
         <v>10020</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>22</v>
@@ -3318,74 +3297,74 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="K16" s="2" t="s">
-        <v>350</v>
+        <v>384</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="115.5" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="129">
       <c r="A17" s="1">
         <v>10021</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="I17" s="2" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="115.5" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="112.9">
       <c r="A18" s="1">
         <v>10023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>23</v>
@@ -3394,36 +3373,36 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>10024</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
@@ -3432,12 +3411,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>10025</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -3446,12 +3425,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>10026</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>26</v>
@@ -3460,12 +3439,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>10027</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>27</v>
@@ -3474,12 +3453,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="145.15">
       <c r="A23" s="1">
         <v>10028</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -3488,36 +3467,36 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="L23" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>10029</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>29</v>
@@ -3526,12 +3505,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>10030</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>30</v>
@@ -3540,12 +3519,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>10031</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>31</v>
@@ -3554,12 +3533,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="132" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="129">
       <c r="A27" s="1">
         <v>10032</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>116</v>
@@ -3571,65 +3550,65 @@
         <v>116</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="115.5" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="112.9">
       <c r="A28" s="1">
         <v>10033</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>358</v>
+        <v>388</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="214.5" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="209.65">
       <c r="A29" s="1">
         <v>10034</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>32</v>
@@ -3638,10 +3617,10 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>114</v>
@@ -3653,21 +3632,21 @@
         <v>115</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="K29" s="2" t="s">
-        <v>360</v>
-      </c>
       <c r="L29" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="96.75">
       <c r="A30" s="1">
         <v>10035</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>33</v>
@@ -3676,30 +3655,30 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>291</v>
+        <v>390</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>362</v>
+        <v>336</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>10036</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>34</v>
@@ -3708,12 +3687,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="145.15">
       <c r="A32" s="1">
         <v>10037</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>35</v>
@@ -3722,74 +3701,74 @@
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>231</v>
+        <v>392</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="145.15">
       <c r="A33" s="1">
         <v>10038</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D33" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>211</v>
+        <v>394</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="66" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="64.5">
       <c r="A34" s="1">
         <v>10039</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>36</v>
@@ -3798,36 +3777,36 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>318</v>
+        <v>397</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="247.5" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="258">
       <c r="A35" s="1">
         <v>10040</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>37</v>
@@ -3836,36 +3815,36 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>368</v>
+        <v>338</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="99" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="96.75">
       <c r="A36" s="1">
         <v>10041</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>38</v>
@@ -3874,36 +3853,36 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>370</v>
+        <v>340</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="145.15">
       <c r="A37" s="1">
         <v>10042</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>39</v>
@@ -3912,36 +3891,36 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>372</v>
+        <v>342</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>10043</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>40</v>
@@ -3950,12 +3929,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="66" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="64.5">
       <c r="A39" s="1">
         <v>10044</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>41</v>
@@ -3964,36 +3943,36 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>374</v>
+        <v>344</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>10045</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>42</v>
@@ -4002,12 +3981,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>10047</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>43</v>
@@ -4016,21 +3995,21 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>10048</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>44</v>
@@ -4039,12 +4018,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>10050</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>45</v>
@@ -4053,12 +4032,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="1">
         <v>10051</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>46</v>
@@ -4067,12 +4046,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="1">
         <v>10052</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>47</v>
@@ -4081,50 +4060,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="149.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="161.25">
       <c r="A46" s="1">
         <v>10054</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D46" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>215</v>
+        <v>398</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="132" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="129">
       <c r="A47" s="1">
         <v>10055</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>48</v>
@@ -4133,36 +4112,36 @@
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>176</v>
+        <v>399</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>378</v>
+        <v>400</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="1">
         <v>10056</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>49</v>
@@ -4171,12 +4150,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="1">
         <v>10057</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>50</v>
@@ -4185,12 +4164,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="1">
         <v>10058</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>51</v>
@@ -4199,50 +4178,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="161.25">
       <c r="A51" s="1">
         <v>10061</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="D51" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>236</v>
+        <v>401</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="1">
         <v>10062</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>52</v>
@@ -4254,12 +4233,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="1">
         <v>10095</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>54</v>
@@ -4268,12 +4247,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="1">
         <v>10096</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>55</v>
@@ -4282,12 +4261,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="1">
         <v>10097</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>56</v>
@@ -4299,50 +4278,50 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="198" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="193.5">
       <c r="A56" s="1">
         <v>10098</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D56" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>169</v>
+        <v>404</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>171</v>
+        <v>405</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>172</v>
+        <v>406</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>380</v>
+        <v>348</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="1">
         <v>10104</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>58</v>
@@ -4351,12 +4330,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="231" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="225.75">
       <c r="A58" s="1">
         <v>10105</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>59</v>
@@ -4365,36 +4344,36 @@
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>382</v>
+        <v>350</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="1">
         <v>10106</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>60</v>
@@ -4403,12 +4382,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" s="1">
         <v>10107</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>61</v>
@@ -4417,12 +4396,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="198" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="193.5">
       <c r="A61" s="1">
         <v>10108</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>62</v>
@@ -4431,33 +4410,33 @@
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="1">
         <v>10109</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>63</v>
@@ -4466,50 +4445,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="247.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="241.9">
       <c r="A63" s="1">
         <v>10202</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D63" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>119</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>387</v>
+        <v>354</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>388</v>
+        <v>355</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="247.5" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="241.9">
       <c r="A64" s="1">
         <v>20012</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>64</v>
@@ -4518,10 +4497,10 @@
         <v>1</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>118</v>
@@ -4530,24 +4509,24 @@
         <v>119</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>387</v>
+        <v>354</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>388</v>
+        <v>355</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="1">
         <v>20014</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>65</v>
@@ -4556,12 +4535,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" s="1">
         <v>20015</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>66</v>
@@ -4570,12 +4549,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" s="1">
         <v>20016</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>57</v>
@@ -4584,12 +4563,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" s="1">
         <v>20017</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>67</v>
@@ -4598,12 +4577,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" s="1">
         <v>20018</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>68</v>
@@ -4612,12 +4591,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" s="1">
         <v>20019</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>69</v>
@@ -4626,12 +4605,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="161.25">
       <c r="A71" s="1">
         <v>30001</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>70</v>
@@ -4640,36 +4619,36 @@
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>390</v>
+        <v>357</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="161.25">
       <c r="A72" s="1">
         <v>30002</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>71</v>
@@ -4678,36 +4657,36 @@
         <v>1</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>392</v>
+        <v>359</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="161.25">
       <c r="A73" s="1">
         <v>30003</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>72</v>
@@ -4716,36 +4695,36 @@
         <v>1</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>270</v>
+        <v>408</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>394</v>
+        <v>361</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="1">
         <v>40003</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>73</v>
@@ -4754,12 +4733,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" s="1">
         <v>40008</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>74</v>
@@ -4768,12 +4747,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" s="1">
         <v>40009</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>75</v>
@@ -4782,12 +4761,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="280.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="290.25">
       <c r="A77" s="1">
         <v>40012</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>76</v>
@@ -4796,36 +4775,36 @@
         <v>1</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G77" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H77" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="I77" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="J77" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J77" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="K77" s="2" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="1">
         <v>40013</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>77</v>
@@ -4834,12 +4813,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" s="1">
         <v>40014</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>78</v>
@@ -4848,12 +4827,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12">
       <c r="A80" s="1">
         <v>40016</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>79</v>
@@ -4862,12 +4841,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12">
       <c r="A81" s="1">
         <v>40017</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>80</v>
@@ -4876,12 +4855,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="231" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="241.9">
       <c r="A82" s="1">
         <v>40018</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>81</v>
@@ -4890,36 +4869,36 @@
         <v>1</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G82" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="I82" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J82" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I82" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J82" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K82" s="2" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="280.5" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="290.25">
       <c r="A83" s="1">
         <v>40019</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>82</v>
@@ -4928,36 +4907,36 @@
         <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G83" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="I83" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J83" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I83" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K83" s="2" t="s">
-        <v>398</v>
+        <v>365</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="231" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="241.9">
       <c r="A84" s="1">
         <v>40020</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>83</v>
@@ -4966,33 +4945,33 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G84" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H84" s="1" t="s">
+      <c r="I84" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J84" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I84" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K84" s="2" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="280.5" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="290.25">
       <c r="A85" s="1">
         <v>40021</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>84</v>
@@ -5001,36 +4980,36 @@
         <v>1</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G85" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H85" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H85" s="1" t="s">
+      <c r="I85" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J85" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I85" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K85" s="2" t="s">
-        <v>398</v>
+        <v>365</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="280.5" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="290.25">
       <c r="A86" s="1">
         <v>40022</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>85</v>
@@ -5039,36 +5018,36 @@
         <v>1</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G86" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H86" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H86" s="1" t="s">
+      <c r="I86" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J86" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I86" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K86" s="2" t="s">
-        <v>398</v>
+        <v>365</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="1">
         <v>40023</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>86</v>
@@ -5077,12 +5056,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="231" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="241.9">
       <c r="A88" s="1">
         <v>40024</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>87</v>
@@ -5091,74 +5070,74 @@
         <v>1</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G88" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H88" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="I88" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J88" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I88" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K88" s="2" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="231" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="241.9">
       <c r="A89" s="1">
         <v>40025</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D89" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>180</v>
+        <v>409</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="1">
         <v>40026</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>88</v>
@@ -5167,12 +5146,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="231" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="241.9">
       <c r="A91" s="1">
         <v>40027</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>89</v>
@@ -5181,36 +5160,36 @@
         <v>1</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G91" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="I91" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J91" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I91" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="K91" s="2" t="s">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="145.15">
       <c r="A92" s="1">
         <v>40028</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>90</v>
@@ -5219,36 +5198,36 @@
         <v>1</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="I92" s="2" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="1">
         <v>40029</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>91</v>
@@ -5257,50 +5236,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="80.650000000000006">
       <c r="A94" s="1">
         <v>40032</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D94" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K94" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D94" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="K94" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="L94" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" ht="66" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="64.5">
       <c r="A95" s="1">
         <v>40034</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>92</v>
@@ -5309,36 +5288,36 @@
         <v>1</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G95" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K95" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H95" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="K95" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="L95" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="1">
         <v>40035</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>93</v>
@@ -5347,12 +5326,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12">
       <c r="A97" s="1">
         <v>50000</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>94</v>
@@ -5361,12 +5340,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12">
       <c r="A98" s="1">
         <v>50001</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>95</v>
@@ -5375,12 +5354,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12">
       <c r="A99" s="1">
         <v>50003</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>96</v>
@@ -5389,12 +5368,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12">
       <c r="A100" s="1">
         <v>90001</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>97</v>
@@ -5403,12 +5382,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12">
       <c r="A101" s="1">
         <v>90011</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>98</v>
@@ -5417,12 +5396,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="132" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="145.15">
       <c r="A102" s="1">
         <v>90017</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>99</v>
@@ -5431,36 +5410,36 @@
         <v>1</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" s="1">
         <v>90019</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>100</v>
@@ -5469,12 +5448,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="161.25">
       <c r="A104" s="1">
         <v>90020</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>101</v>
@@ -5483,36 +5462,36 @@
         <v>1</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G104" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K104" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="H104" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="L104" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="1">
         <v>90021</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>102</v>
@@ -5521,12 +5500,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="132" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="129">
       <c r="A106" s="1">
         <v>90022</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>103</v>
@@ -5535,36 +5514,36 @@
         <v>1</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>408</v>
+        <v>373</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" s="1">
         <v>90023</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>104</v>
@@ -5573,12 +5552,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="145.15">
       <c r="A108" s="1">
         <v>90024</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>105</v>
@@ -5587,36 +5566,36 @@
         <v>1</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G108" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J108" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H108" s="1" t="s">
+      <c r="K108" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="I108" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="L108" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" s="1">
         <v>90025</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>106</v>
@@ -5625,12 +5604,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12">
       <c r="A110" s="1">
         <v>90026</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>107</v>
@@ -5639,12 +5618,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="66" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="80.650000000000006">
       <c r="A111" s="1">
         <v>90027</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>108</v>
@@ -5653,36 +5632,36 @@
         <v>1</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>330</v>
+        <v>412</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" s="1">
         <v>90028</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>109</v>
@@ -5691,12 +5670,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12">
       <c r="A113" s="1">
         <v>90029</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>110</v>
@@ -5705,12 +5684,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12">
       <c r="A114" s="1">
         <v>90030</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>111</v>
@@ -5719,12 +5698,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12">
       <c r="A115" s="1">
         <v>90033</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>112</v>
@@ -5733,12 +5712,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="115.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="112.9">
       <c r="A116" s="1">
         <v>90034</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>113</v>
@@ -5747,28 +5726,28 @@
         <v>1</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G116" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J116" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H116" s="1" t="s">
+      <c r="K116" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I116" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J116" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="L116" s="2" t="s">
-        <v>412</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>